<commit_message>
Completes the testing of defillama_slugs
Defillama_slugs was updated for unit testing returns and also
simplification of data access using the data for a single
Defillama listing instead of the entire list of lists of all
Defillama lists, so these changes required re-running the
test cases.
</commit_message>
<xml_diff>
--- a/test/crypto_valuation_test_cases_V1.1.xlsx
+++ b/test/crypto_valuation_test_cases_V1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\My Drive\Documents_Google_Drive\Career_Folder\Quant_Trading_Version_2.0\Learning\Crypto\crypto_valuation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADE5FB6-3FCB-412C-ACA2-8D5CFCC34E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE4A77A-675F-49F7-AA8B-15C371C30C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6F403E5E-B41C-4F60-9A95-EB5DE25D92E4}"/>
+    <workbookView xWindow="15" yWindow="255" windowWidth="26655" windowHeight="14835" activeTab="1" xr2:uid="{6F403E5E-B41C-4F60-9A95-EB5DE25D92E4}"/>
   </bookViews>
   <sheets>
     <sheet name="configs.py" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
   <si>
     <t>Project Name</t>
   </si>
@@ -643,18 +643,12 @@
     <t>All listings with a not NA defillama slug has a TVL. Note, some TVLs are actually 0. Ex: ETC and Bepswap.</t>
   </si>
   <si>
-    <t xml:space="preserve">The 0 TVLs are actually zero. </t>
-  </si>
-  <si>
     <t xml:space="preserve">All listings with defillama_slug = NA should also have NA for TVLs. </t>
   </si>
   <si>
     <t>If Defillama cmcId has a value, the corresponding CMC ID should be the same.</t>
   </si>
   <si>
-    <t>A formula check on the two CMC IDs agrees.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test that defillama_slug correctly puts only listings that do not have a Defillama cmcId but has a valid Defillama slug in the NA category (listed on Defillama but not not listed on CMC). </t>
   </si>
   <si>
@@ -704,6 +698,15 @@
   </si>
   <si>
     <t xml:space="preserve">The ID_REQUEST_LENGTH of 2000 should result in a 4xx response from the quotes/latest endupoint. </t>
+  </si>
+  <si>
+    <t>The 0 TVLs are actually zero. Re-tested on 27-Jan-22 after updates a) unit testing and b) using defillama_protocol instead defillama_protocols[i].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-tested because of the updates above. </t>
+  </si>
+  <si>
+    <t>For every cmcID that can be found on Coinmarketcap, the code mapped the Defillama listing to the Coinmarketcap listing, but there are Defillama listings with cmcIds that cannot be found on Coinmarketcap. See the PDF attachment to the right.</t>
   </si>
 </sst>
 </file>
@@ -803,6 +806,79 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>11206</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>571499</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>27</xdr:col>
+          <xdr:colOff>195744</xdr:colOff>
+          <xdr:row>58</xdr:row>
+          <xdr:rowOff>67235</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2091" name="Object 43" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2091"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E96FB2BD-7E15-419A-9485-C6996356F535}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1104,9 +1180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82E5239-E1B1-48D9-BDAE-76F9EC50F24D}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1297,7 @@
         <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>23</v>
@@ -1542,9 +1618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC2C759-EFF8-4AA5-9213-C4DF14F32BC8}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,12 +1753,12 @@
       </c>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>26</v>
@@ -1706,10 +1782,10 @@
         <v>32</v>
       </c>
       <c r="J10" s="7">
-        <v>44587</v>
+        <v>44588</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1726,7 +1802,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>31</v>
@@ -1738,11 +1814,13 @@
         <v>32</v>
       </c>
       <c r="J11" s="7">
-        <v>44587</v>
-      </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>44588</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1756,7 +1834,7 @@
         <v>41</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>31</v>
@@ -1768,10 +1846,10 @@
         <v>32</v>
       </c>
       <c r="J12" s="7">
-        <v>44587</v>
+        <v>44588</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1782,13 +1860,13 @@
         <v>29</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>31</v>
@@ -1800,16 +1878,18 @@
         <v>32</v>
       </c>
       <c r="J13" s="7">
-        <v>44587</v>
-      </c>
-      <c r="K13" s="3"/>
+        <v>44588</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>30</v>
@@ -1821,7 +1901,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>31</v>
@@ -1842,19 +1922,19 @@
         <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>31</v>
@@ -1878,13 +1958,13 @@
         <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>31</v>
@@ -1905,16 +1985,16 @@
         <v>46</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>31</v>
@@ -1936,16 +2016,16 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>31</v>
@@ -2146,6 +2226,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Acrobat.Document.DC" shapeId="2091" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>12</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>571500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>27</xdr:col>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>58</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Acrobat.Document.DC" shapeId="2091" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Merge Version_1.1_Development branch into master
This commit merges the changes from V1.1 into master. Version 1.0
is deprecated.
</commit_message>
<xml_diff>
--- a/test/crypto_valuation_test_cases_V1.1.xlsx
+++ b/test/crypto_valuation_test_cases_V1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\My Drive\Documents_Google_Drive\Career_Folder\Quant_Trading_Version_2.0\Learning\Crypto\crypto_valuation\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE4A77A-675F-49F7-AA8B-15C371C30C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D4312B-2F84-45A7-BBEE-DB10CCECDDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="255" windowWidth="26655" windowHeight="14835" activeTab="1" xr2:uid="{6F403E5E-B41C-4F60-9A95-EB5DE25D92E4}"/>
   </bookViews>
@@ -815,15 +815,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
-          <xdr:colOff>11206</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>571499</xdr:rowOff>
+          <xdr:rowOff>571500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>27</xdr:col>
-          <xdr:colOff>195744</xdr:colOff>
+          <xdr:colOff>200025</xdr:colOff>
           <xdr:row>58</xdr:row>
-          <xdr:rowOff>67235</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -833,7 +833,7 @@
                   <a14:compatExt spid="_x0000_s2091"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E96FB2BD-7E15-419A-9485-C6996356F535}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -854,23 +854,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1620,7 +1607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>